<commit_message>
green line excel and visual widget added using formatted json placement data, removed branch parameter from track block.
</commit_message>
<xml_diff>
--- a/tests/blue_line.xlsx
+++ b/tests/blue_line.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0c4a204f81830ef/Pitt/2024_Summer_Term/ECE 1140/Project/train_system/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94040FE2-6B3D-4D76-8A07-97B1A1A6E701}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CBEE126-31A2-45F2-8B0F-084D292D7231}"/>
   <bookViews>
-    <workbookView xWindow="-33840" yWindow="4560" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
   <si>
     <t>Line</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>Station</t>
-  </si>
-  <si>
-    <t>Branch</t>
   </si>
 </sst>
 </file>
@@ -470,28 +467,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.81640625" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" customWidth="1"/>
-    <col min="10" max="10" width="13.81640625" customWidth="1"/>
-    <col min="11" max="11" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="32.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -513,23 +510,20 @@
       <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>28</v>
+      <c r="H1" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="J1" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="K1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -551,19 +545,16 @@
       <c r="G2" s="2">
         <v>2</v>
       </c>
-      <c r="H2" s="2">
-        <v>1</v>
-      </c>
+      <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="J2" s="6">
+        <v>0</v>
+      </c>
       <c r="K2" s="6">
         <v>0</v>
       </c>
-      <c r="L2" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -585,19 +576,16 @@
       <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
+      <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
       <c r="K3" s="6">
         <v>0</v>
       </c>
-      <c r="L3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -619,19 +607,16 @@
       <c r="G4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
+      <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
       <c r="K4" s="6">
         <v>0</v>
       </c>
-      <c r="L4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -653,19 +638,16 @@
       <c r="G5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
+      <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="J5" s="6">
+        <v>0</v>
+      </c>
       <c r="K5" s="6">
         <v>0</v>
       </c>
-      <c r="L5" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -687,19 +669,16 @@
       <c r="G6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
+      <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="J6" s="6">
+        <v>0</v>
+      </c>
       <c r="K6" s="6">
         <v>0</v>
       </c>
-      <c r="L6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -721,19 +700,16 @@
       <c r="G7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
+      <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="J7" s="6">
+        <v>0</v>
+      </c>
       <c r="K7" s="6">
         <v>0</v>
       </c>
-      <c r="L7" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -755,19 +731,16 @@
       <c r="G8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="2">
-        <v>1</v>
-      </c>
+      <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="J8" s="6">
+        <v>0</v>
+      </c>
       <c r="K8" s="6">
         <v>0</v>
       </c>
-      <c r="L8" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -789,19 +762,16 @@
       <c r="G9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="2">
-        <v>1</v>
-      </c>
+      <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="J9" s="6">
+        <v>0</v>
+      </c>
       <c r="K9" s="6">
         <v>0</v>
       </c>
-      <c r="L9" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -823,19 +793,16 @@
       <c r="G10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="2">
-        <v>1</v>
-      </c>
+      <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="J10" s="6">
+        <v>0</v>
+      </c>
       <c r="K10" s="6">
         <v>0</v>
       </c>
-      <c r="L10" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -857,23 +824,20 @@
       <c r="G11" s="2">
         <v>9</v>
       </c>
-      <c r="H11" s="2">
-        <v>1</v>
+      <c r="H11" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="J11" s="6">
+        <v>0</v>
+      </c>
       <c r="K11" s="6">
         <v>0</v>
       </c>
-      <c r="L11" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -895,19 +859,16 @@
       <c r="G12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="2">
-        <v>0</v>
-      </c>
+      <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="J12" s="6">
+        <v>0</v>
+      </c>
       <c r="K12" s="6">
         <v>0</v>
       </c>
-      <c r="L12" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -929,19 +890,16 @@
       <c r="G13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="2">
-        <v>0</v>
-      </c>
+      <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="J13" s="6">
+        <v>0</v>
+      </c>
       <c r="K13" s="6">
         <v>0</v>
       </c>
-      <c r="L13" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -963,19 +921,16 @@
       <c r="G14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="2">
-        <v>0</v>
-      </c>
+      <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="J14" s="6">
+        <v>0</v>
+      </c>
       <c r="K14" s="6">
         <v>0</v>
       </c>
-      <c r="L14" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -997,19 +952,16 @@
       <c r="G15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="2">
-        <v>0</v>
-      </c>
+      <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="J15" s="6">
+        <v>0</v>
+      </c>
       <c r="K15" s="6">
         <v>0</v>
       </c>
-      <c r="L15" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1031,19 +983,16 @@
       <c r="G16" s="2">
         <v>14</v>
       </c>
-      <c r="H16" s="2">
-        <v>0</v>
+      <c r="H16" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J16" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="J16" s="6">
+        <v>0</v>
+      </c>
       <c r="K16" s="6">
-        <v>0</v>
-      </c>
-      <c r="L16" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>